<commit_message>
add Full Basic Math/Rom Board
</commit_message>
<xml_diff>
--- a/notes/ASCII-KEYBOARD/Netronics-ASCII-Keyboard-BOM.xlsx
+++ b/notes/ASCII-KEYBOARD/Netronics-ASCII-Keyboard-BOM.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwasson/Development/avi-elf-ii/notes/ASCII-KEYBOARD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89CB8ADE-F30B-DF49-A307-5AB7BD5D5179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910C6C75-7557-4045-BBB7-DEE2FCD7FA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="3240" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22520" yWindow="4360" windowWidth="37060" windowHeight="23660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Netronics ASCII Keyboard" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="125">
   <si>
     <t>Qty</t>
   </si>
@@ -238,9 +251,6 @@
     <t>Regulator_Linear:LM7912_TO220</t>
   </si>
   <si>
-    <t>hhttps://www.onsemi.com/pub/Collateral/MC7900-D.PDF</t>
-  </si>
-  <si>
     <t xml:space="preserve">Momentary Pushbutton </t>
   </si>
   <si>
@@ -313,30 +323,15 @@
     <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CF14JT1K00/1741314</t>
   </si>
   <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>No R5.</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/omron-electronics-inc-emc-div/G5V-2-DC5/87819</t>
   </si>
   <si>
     <t xml:space="preserve">Keyboard Encoder Chip. </t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/stmicroelectronics/2N3904/603420</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/sunled/XLUR12D/4745846</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/smc-diode-solutions/1N4001/5992908</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PREC040SAAN-RC/2774814</t>
   </si>
   <si>
@@ -380,6 +375,39 @@
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CF14JT680R/1741489</t>
+  </si>
+  <si>
+    <t>Stiffeners</t>
+  </si>
+  <si>
+    <t>Keyboard Stiffeners for space bar</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/540-0G990743</t>
+  </si>
+  <si>
+    <t>540-0G990743</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pub/Collateral/MC7900-D.PDF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/onsemi/2N3904BU/1413</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/onsemi/1N4001RLG/917621</t>
+  </si>
+  <si>
+    <t>Keycaps</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JLCPCB $66.52 CAD for 5 boards </t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/</t>
   </si>
 </sst>
 </file>
@@ -1235,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1247,6 +1275,7 @@
     <col min="3" max="3" width="17.1640625" customWidth="1"/>
     <col min="4" max="4" width="31.1640625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="86.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1260,7 +1289,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1269,58 +1298,26 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" t="s">
-        <v>83</v>
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1328,147 +1325,147 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
         <v>69</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>70</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D7" t="s">
         <v>71</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E7" t="s">
         <v>67</v>
       </c>
-      <c r="F5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" t="s">
-        <v>103</v>
+      <c r="F7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D12" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E12" t="s">
         <v>30</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F12" t="s">
         <v>31</v>
       </c>
-      <c r="G10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" t="s">
-        <v>111</v>
+      <c r="G12" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1476,22 +1473,22 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
       </c>
-      <c r="G15" t="s">
-        <v>107</v>
+      <c r="G15" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1499,10 +1496,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -1513,19 +1510,19 @@
       <c r="F16" t="s">
         <v>9</v>
       </c>
-      <c r="G16" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G16" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
@@ -1536,42 +1533,42 @@
       <c r="F17" t="s">
         <v>9</v>
       </c>
-      <c r="G17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G17" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F18" t="s">
         <v>9</v>
       </c>
-      <c r="G18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G18" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -1582,66 +1579,70 @@
       <c r="F19" t="s">
         <v>9</v>
       </c>
-      <c r="G19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="G19" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
         <v>9</v>
       </c>
-      <c r="G23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G20" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D24" t="s">
         <v>51</v>
@@ -1653,18 +1654,18 @@
         <v>9</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
         <v>51</v>
@@ -1676,18 +1677,18 @@
         <v>9</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D26" t="s">
         <v>51</v>
@@ -1698,19 +1699,19 @@
       <c r="F26" t="s">
         <v>9</v>
       </c>
-      <c r="G26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G26" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
         <v>51</v>
@@ -1721,19 +1722,19 @@
       <c r="F27" t="s">
         <v>9</v>
       </c>
-      <c r="G27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G27" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D28" t="s">
         <v>51</v>
@@ -1744,19 +1745,19 @@
       <c r="F28" t="s">
         <v>9</v>
       </c>
-      <c r="G28" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G28" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D29" t="s">
         <v>51</v>
@@ -1767,19 +1768,19 @@
       <c r="F29" t="s">
         <v>9</v>
       </c>
-      <c r="G29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G29" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
         <v>51</v>
@@ -1790,87 +1791,73 @@
       <c r="F30" t="s">
         <v>9</v>
       </c>
-      <c r="G30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="G30" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>55</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>103</v>
+      </c>
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>121</v>
+      </c>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="37" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>109</v>
-      </c>
-      <c r="E33" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" t="s">
-        <v>43</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G36" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" t="s">
-        <v>106</v>
-      </c>
-      <c r="E37" t="s">
-        <v>35</v>
-      </c>
-      <c r="F37" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1878,22 +1865,22 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="E38" t="s">
-        <v>35</v>
-      </c>
-      <c r="F38" t="s">
-        <v>9</v>
+        <v>43</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1901,13 +1888,13 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D39" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E39" t="s">
         <v>35</v>
@@ -1915,18 +1902,107 @@
       <c r="F39" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>105</v>
+      <c r="G39" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" t="s">
+        <v>100</v>
+      </c>
+      <c r="E40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" t="s">
+        <v>115</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F36" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G37" r:id="rId2" xr:uid="{395A816A-63B4-3F47-A4F3-285A5CE7A0B9}"/>
-    <hyperlink ref="G38" r:id="rId3" xr:uid="{9234BD1D-29E2-5846-AC07-9A1A6C4747C8}"/>
-    <hyperlink ref="G39" r:id="rId4" xr:uid="{18255DF7-368B-2947-A8B9-C475A4281543}"/>
-    <hyperlink ref="G24" r:id="rId5" xr:uid="{C05A123C-DE60-7340-B47C-3545F0643542}"/>
-    <hyperlink ref="G25" r:id="rId6" xr:uid="{525200EA-CF80-764E-B67A-8268BFCAFBF5}"/>
+    <hyperlink ref="F38" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G39" r:id="rId2" xr:uid="{395A816A-63B4-3F47-A4F3-285A5CE7A0B9}"/>
+    <hyperlink ref="G40" r:id="rId3" xr:uid="{9234BD1D-29E2-5846-AC07-9A1A6C4747C8}"/>
+    <hyperlink ref="G41" r:id="rId4" xr:uid="{18255DF7-368B-2947-A8B9-C475A4281543}"/>
+    <hyperlink ref="G25" r:id="rId5" xr:uid="{C05A123C-DE60-7340-B47C-3545F0643542}"/>
+    <hyperlink ref="G26" r:id="rId6" xr:uid="{525200EA-CF80-764E-B67A-8268BFCAFBF5}"/>
+    <hyperlink ref="G42" r:id="rId7" xr:uid="{FA8571A4-72A4-AF44-9763-2CDF6EB36E18}"/>
+    <hyperlink ref="G15" r:id="rId8" xr:uid="{E5B97F73-F31D-034F-AB51-2C0B03A44121}"/>
+    <hyperlink ref="G16" r:id="rId9" xr:uid="{41E3A1E5-A582-0A46-B7BA-91919CBA3A91}"/>
+    <hyperlink ref="G17" r:id="rId10" xr:uid="{AC830B4B-5D65-9545-A0F1-524C93F25F73}"/>
+    <hyperlink ref="G18" r:id="rId11" xr:uid="{D34E0840-53AB-AF42-A221-872BA0E954FE}"/>
+    <hyperlink ref="G19" r:id="rId12" xr:uid="{7CCE1818-A6AB-6B49-BE37-004F9C114849}"/>
+    <hyperlink ref="G20" r:id="rId13" xr:uid="{68E88992-A97A-4B44-9CC5-DAFFB5550031}"/>
+    <hyperlink ref="G21" r:id="rId14" xr:uid="{683CC22E-815F-954D-A2FC-9B31FE73A557}"/>
+    <hyperlink ref="G24" r:id="rId15" xr:uid="{69BCA6B4-918A-724B-881D-0A53CC54B5B7}"/>
+    <hyperlink ref="G27" r:id="rId16" xr:uid="{5BE22161-1CE9-C545-BD6A-5EAD92D7D17E}"/>
+    <hyperlink ref="G28" r:id="rId17" xr:uid="{AED0FB29-4702-8B40-AC6E-F75CC4A4850E}"/>
+    <hyperlink ref="G29" r:id="rId18" xr:uid="{55565B9B-4EAA-8841-A1A2-15F34CE3BA93}"/>
+    <hyperlink ref="G30" r:id="rId19" xr:uid="{303B29A5-9171-A842-9163-51AED76794C8}"/>
+    <hyperlink ref="G31" r:id="rId20" xr:uid="{4C33FFB1-7526-294D-916B-DCDF4962C953}"/>
+    <hyperlink ref="G34" r:id="rId21" xr:uid="{B5EE27F2-2564-904D-9731-CBB256A7E288}"/>
+    <hyperlink ref="G38" r:id="rId22" xr:uid="{84E949A2-7427-9740-816F-1DF2F772CC34}"/>
+    <hyperlink ref="F5" r:id="rId23" xr:uid="{AE97028B-7565-A64A-BFFE-542B07A29CCD}"/>
+    <hyperlink ref="G5" r:id="rId24" xr:uid="{D04F5BBC-58C5-7246-8671-EFD263B8A094}"/>
+    <hyperlink ref="G6" r:id="rId25" xr:uid="{4638D723-4F7C-C841-B081-28B9BF8145BB}"/>
+    <hyperlink ref="G7" r:id="rId26" xr:uid="{DAD9A993-A6F8-A549-91C4-8B4E53F6697F}"/>
+    <hyperlink ref="F6" r:id="rId27" xr:uid="{81A7AF17-AD97-884D-A29A-46789A7614E2}"/>
+    <hyperlink ref="F7" r:id="rId28" xr:uid="{9EA75995-0C95-C846-84A3-A9E26BB9A63E}"/>
+    <hyperlink ref="G10" r:id="rId29" xr:uid="{03E249B5-22BC-F844-A533-60F01FE5814A}"/>
+    <hyperlink ref="G11" r:id="rId30" xr:uid="{EF6A6A15-57FF-1A40-ABE1-E46A9D52B206}"/>
+    <hyperlink ref="G12" r:id="rId31" xr:uid="{FF1292D1-7DD2-4247-AD24-BC9D4E1A5BEF}"/>
+    <hyperlink ref="G2" r:id="rId32" xr:uid="{D2A344DA-6685-6A45-B404-C278E7D56318}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>